<commit_message>
Corrected J assignment (typo in ASD)
</commit_message>
<xml_diff>
--- a/calculations/Pb_I/fit_Rydberg.xlsx
+++ b/calculations/Pb_I/fit_Rydberg.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://nistgov-my.sharepoint.com/personal/irikura_nist_gov/Documents/Karl/atomic_SOC/calculations/Pb_I/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="869" documentId="11_F25DC773A252ABDACC1048BFA95E751A5BDE58F9" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{8008B3DE-68E5-4C58-9210-C9FAB02CAD3C}"/>
+  <xr:revisionPtr revIDLastSave="1063" documentId="11_F25DC773A252ABDACC1048BFA95E751A5BDE58F9" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{8A3CA6D3-CFB1-4115-9DA5-A34862FAADC9}"/>
   <bookViews>
     <workbookView xWindow="-25320" yWindow="1725" windowWidth="25440" windowHeight="15390" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -18,7 +18,7 @@
   <definedNames>
     <definedName name="IE">Sheet1!$F$1</definedName>
     <definedName name="Rhc">Sheet1!$K$1</definedName>
-    <definedName name="solver_adj" localSheetId="0" hidden="1">Sheet1!$Q$4</definedName>
+    <definedName name="solver_adj" localSheetId="0" hidden="1">Sheet1!$P$4</definedName>
     <definedName name="solver_cvg" localSheetId="0" hidden="1">0.0001</definedName>
     <definedName name="solver_drv" localSheetId="0" hidden="1">1</definedName>
     <definedName name="solver_eng" localSheetId="0" hidden="1">1</definedName>
@@ -32,7 +32,7 @@
     <definedName name="solver_nod" localSheetId="0" hidden="1">2147483647</definedName>
     <definedName name="solver_num" localSheetId="0" hidden="1">0</definedName>
     <definedName name="solver_nwt" localSheetId="0" hidden="1">1</definedName>
-    <definedName name="solver_opt" localSheetId="0" hidden="1">Sheet1!$Q$13</definedName>
+    <definedName name="solver_opt" localSheetId="0" hidden="1">Sheet1!$P$13</definedName>
     <definedName name="solver_pre" localSheetId="0" hidden="1">0.000001</definedName>
     <definedName name="solver_rbv" localSheetId="0" hidden="1">1</definedName>
     <definedName name="solver_rlx" localSheetId="0" hidden="1">2</definedName>
@@ -67,7 +67,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="32">
   <si>
     <t>Fit levels to Rydberg equation</t>
   </si>
@@ -160,6 +160,9 @@
   </si>
   <si>
     <t>Fit each series</t>
+  </si>
+  <si>
+    <t>typo in ASD</t>
   </si>
 </sst>
 </file>
@@ -350,7 +353,7 @@
                   <c:v>4891.4779999999955</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>3351.8479999999981</c:v>
+                  <c:v>3344.4179999999978</c:v>
                 </c:pt>
                 <c:pt idx="4">
                   <c:v>2389.8580000000002</c:v>
@@ -436,25 +439,25 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="7"/>
                 <c:pt idx="0">
-                  <c:v>15073.302869920377</c:v>
+                  <c:v>15072.646786092686</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>8023.7109007734571</c:v>
+                  <c:v>8023.4560925520036</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>4971.5600784638173</c:v>
+                  <c:v>4971.4358011757777</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>3379.714986680352</c:v>
+                  <c:v>3379.6453281552467</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>2445.9020724898164</c:v>
+                  <c:v>2445.8591866658753</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>1851.7262494720326</c:v>
+                  <c:v>1851.6979993012762</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>1450.4283799293994</c:v>
+                  <c:v>1450.4087959516412</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1283,6 +1286,10 @@
 </xdr:wsDr>
 </file>
 
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
+</file>
+
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
 <a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
@@ -1549,7 +1556,7 @@
   <dimension ref="A1:V31"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D6" sqref="D6"/>
+      <selection activeCell="U9" sqref="U9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1615,10 +1622,10 @@
         <v>4.3271297285038495</v>
       </c>
       <c r="P4">
-        <v>4.3018073587870216</v>
+        <v>4.3017486358129604</v>
       </c>
       <c r="Q4">
-        <v>4.2917499917405619</v>
+        <v>4.2918096623756661</v>
       </c>
       <c r="S4" t="s">
         <v>29</v>
@@ -1694,7 +1701,7 @@
         <v>42918.64</v>
       </c>
       <c r="E6" s="4">
-        <f>IE-D6</f>
+        <f t="shared" ref="E6:E31" si="0">IE-D6</f>
         <v>16900.917999999998</v>
       </c>
       <c r="H6">
@@ -1717,36 +1724,36 @@
         <v>15010.197999999997</v>
       </c>
       <c r="N6">
-        <f>Rhc/($H6-N$4)^2</f>
+        <f t="shared" ref="N6:Q11" si="1">Rhc/($H6-N$4)^2</f>
         <v>16801.227029328609</v>
       </c>
       <c r="O6">
-        <f>Rhc/($H6-O$4)^2</f>
+        <f t="shared" si="1"/>
         <v>15360.260151188357</v>
       </c>
       <c r="P6">
-        <f>Rhc/($H6-P$4)^2</f>
-        <v>15073.302869920377</v>
+        <f t="shared" si="1"/>
+        <v>15072.646786092686</v>
       </c>
       <c r="Q6">
-        <f>Rhc/($H6-Q$4)^2</f>
-        <v>14961.558199268686</v>
+        <f t="shared" si="1"/>
+        <v>14962.217514459961</v>
       </c>
       <c r="S6" s="4">
         <f>N6-I6</f>
         <v>-99.690970671388641</v>
       </c>
       <c r="T6" s="4">
-        <f t="shared" ref="T6:T13" si="0">O6-J6</f>
+        <f t="shared" ref="T6:T11" si="2">O6-J6</f>
         <v>-58.407848811641088</v>
       </c>
       <c r="U6" s="4">
-        <f t="shared" ref="U6:U13" si="1">P6-K6</f>
-        <v>-71.265130079622395</v>
+        <f t="shared" ref="U6:U12" si="3">P6-K6</f>
+        <v>-71.921213907313359</v>
       </c>
       <c r="V6" s="4">
-        <f t="shared" ref="V6:V13" si="2">Q6-L6</f>
-        <v>-48.63980073131097</v>
+        <f t="shared" ref="V6:V12" si="4">Q6-L6</f>
+        <v>-47.98048554003617</v>
       </c>
     </row>
     <row r="7" spans="1:22" x14ac:dyDescent="0.25">
@@ -1757,7 +1764,7 @@
         <v>44400.89</v>
       </c>
       <c r="E7" s="4">
-        <f>IE-D7</f>
+        <f t="shared" si="0"/>
         <v>15418.667999999998</v>
       </c>
       <c r="H7">
@@ -1780,36 +1787,36 @@
         <v>7875.4479999999967</v>
       </c>
       <c r="N7">
-        <f>Rhc/($H7-N$4)^2</f>
+        <f t="shared" si="1"/>
         <v>8679.7800287088339</v>
       </c>
       <c r="O7">
-        <f>Rhc/($H7-O$4)^2</f>
+        <f t="shared" si="1"/>
         <v>8134.730219439185</v>
       </c>
       <c r="P7">
-        <f>Rhc/($H7-P$4)^2</f>
-        <v>8023.7109007734571</v>
+        <f t="shared" si="1"/>
+        <v>8023.4560925520036</v>
       </c>
       <c r="Q7">
-        <f>Rhc/($H7-Q$4)^2</f>
-        <v>7980.2467474452333</v>
+        <f t="shared" si="1"/>
+        <v>7980.5035790421298</v>
       </c>
       <c r="S7" s="4">
-        <f t="shared" ref="S7:S13" si="3">N7-I7</f>
+        <f t="shared" ref="S7:S11" si="5">N7-I7</f>
         <v>180.82202870883521</v>
       </c>
       <c r="T7" s="4">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>101.23221943918543</v>
       </c>
       <c r="U7" s="4">
-        <f t="shared" si="1"/>
-        <v>121.09290077346213</v>
+        <f t="shared" si="3"/>
+        <v>120.83809255200867</v>
       </c>
       <c r="V7" s="4">
-        <f t="shared" si="2"/>
-        <v>104.79874744523659</v>
+        <f t="shared" si="4"/>
+        <v>105.0555790421331</v>
       </c>
     </row>
     <row r="8" spans="1:22" x14ac:dyDescent="0.25">
@@ -1823,7 +1830,7 @@
         <v>44674.99</v>
       </c>
       <c r="E8" s="4">
-        <f>IE-D8</f>
+        <f t="shared" si="0"/>
         <v>15144.567999999999</v>
       </c>
       <c r="H8">
@@ -1846,36 +1853,36 @@
         <v>4889.4479999999967</v>
       </c>
       <c r="N8">
-        <f>Rhc/($H8-N$4)^2</f>
+        <f t="shared" si="1"/>
         <v>5287.4673158898249</v>
       </c>
       <c r="O8">
-        <f>Rhc/($H8-O$4)^2</f>
+        <f t="shared" si="1"/>
         <v>5025.5880226223853</v>
       </c>
       <c r="P8">
-        <f>Rhc/($H8-P$4)^2</f>
-        <v>4971.5600784638173</v>
+        <f t="shared" si="1"/>
+        <v>4971.4358011757777</v>
       </c>
       <c r="Q8">
-        <f>Rhc/($H8-Q$4)^2</f>
-        <v>4950.3431079708525</v>
+        <f t="shared" si="1"/>
+        <v>4950.4685880249326</v>
       </c>
       <c r="S8" s="4">
+        <f t="shared" si="5"/>
+        <v>121.62931588982883</v>
+      </c>
+      <c r="T8" s="4">
+        <f t="shared" si="2"/>
+        <v>67.840022622385732</v>
+      </c>
+      <c r="U8" s="4">
         <f t="shared" si="3"/>
-        <v>121.62931588982883</v>
-      </c>
-      <c r="T8" s="4">
-        <f t="shared" si="0"/>
-        <v>67.840022622385732</v>
-      </c>
-      <c r="U8" s="4">
-        <f t="shared" si="1"/>
-        <v>80.082078463821745</v>
+        <v>79.957801175782151</v>
       </c>
       <c r="V8" s="4">
-        <f t="shared" si="2"/>
-        <v>60.895107970855861</v>
+        <f t="shared" si="4"/>
+        <v>61.020588024935932</v>
       </c>
     </row>
     <row r="9" spans="1:22" x14ac:dyDescent="0.25">
@@ -1886,7 +1893,7 @@
         <v>44809.36</v>
       </c>
       <c r="E9" s="4">
-        <f>IE-D9</f>
+        <f t="shared" si="0"/>
         <v>15010.197999999997</v>
       </c>
       <c r="H9">
@@ -1901,44 +1908,44 @@
         <v>3368.5279999999984</v>
       </c>
       <c r="K9" s="4">
+        <f>E21</f>
+        <v>3344.4179999999978</v>
+      </c>
+      <c r="L9" s="4">
         <f>E20</f>
         <v>3351.8479999999981</v>
       </c>
-      <c r="L9" s="4">
-        <f>E21</f>
-        <v>3344.4179999999978</v>
-      </c>
       <c r="N9">
-        <f>Rhc/($H9-N$4)^2</f>
+        <f t="shared" si="1"/>
         <v>3555.3283028820415</v>
       </c>
       <c r="O9">
-        <f>Rhc/($H9-O$4)^2</f>
+        <f t="shared" si="1"/>
         <v>3409.9548470135669</v>
       </c>
       <c r="P9">
-        <f>Rhc/($H9-P$4)^2</f>
-        <v>3379.714986680352</v>
+        <f t="shared" si="1"/>
+        <v>3379.6453281552467</v>
       </c>
       <c r="Q9">
-        <f>Rhc/($H9-Q$4)^2</f>
-        <v>3367.8160370272126</v>
+        <f t="shared" si="1"/>
+        <v>3367.8864484046635</v>
       </c>
       <c r="S9" s="4">
+        <f t="shared" si="5"/>
+        <v>74.700302882044525</v>
+      </c>
+      <c r="T9" s="4">
+        <f t="shared" si="2"/>
+        <v>41.426847013568477</v>
+      </c>
+      <c r="U9" s="4">
         <f t="shared" si="3"/>
-        <v>74.700302882044525</v>
-      </c>
-      <c r="T9" s="4">
-        <f t="shared" si="0"/>
-        <v>41.426847013568477</v>
-      </c>
-      <c r="U9" s="4">
-        <f t="shared" si="1"/>
-        <v>27.866986680353875</v>
+        <v>35.22732815524887</v>
       </c>
       <c r="V9" s="4">
-        <f t="shared" si="2"/>
-        <v>23.398037027214741</v>
+        <f t="shared" si="4"/>
+        <v>16.03844840466536</v>
       </c>
     </row>
     <row r="10" spans="1:22" x14ac:dyDescent="0.25">
@@ -1955,7 +1962,7 @@
         <v>51320.6</v>
       </c>
       <c r="E10" s="4">
-        <f>IE-D10</f>
+        <f t="shared" si="0"/>
         <v>8498.9579999999987</v>
       </c>
       <c r="H10">
@@ -1978,36 +1985,36 @@
         <v>2558.887999999999</v>
       </c>
       <c r="N10">
-        <f>Rhc/($H10-N$4)^2</f>
+        <f t="shared" si="1"/>
         <v>2553.3990373294382</v>
       </c>
       <c r="O10">
-        <f>Rhc/($H10-O$4)^2</f>
+        <f t="shared" si="1"/>
         <v>2464.5008320136203</v>
       </c>
       <c r="P10">
-        <f>Rhc/($H10-P$4)^2</f>
-        <v>2445.9020724898164</v>
+        <f t="shared" si="1"/>
+        <v>2445.8591866658753</v>
       </c>
       <c r="Q10">
-        <f>Rhc/($H10-Q$4)^2</f>
-        <v>2438.5735159949159</v>
+        <f t="shared" si="1"/>
+        <v>2438.6168993428237</v>
       </c>
       <c r="S10" s="4">
+        <f t="shared" si="5"/>
+        <v>51.681037329437459</v>
+      </c>
+      <c r="T10" s="4">
+        <f t="shared" si="2"/>
+        <v>25.822832013620427</v>
+      </c>
+      <c r="U10" s="4">
         <f t="shared" si="3"/>
-        <v>51.681037329437459</v>
-      </c>
-      <c r="T10" s="4">
-        <f t="shared" si="0"/>
-        <v>25.822832013620427</v>
-      </c>
-      <c r="U10" s="4">
-        <f t="shared" si="1"/>
-        <v>56.044072489816244</v>
+        <v>56.001186665875139</v>
       </c>
       <c r="V10" s="4">
-        <f t="shared" si="2"/>
-        <v>-120.31448400508316</v>
+        <f t="shared" si="4"/>
+        <v>-120.27110065717534</v>
       </c>
     </row>
     <row r="11" spans="1:22" x14ac:dyDescent="0.25">
@@ -2018,7 +2025,7 @@
         <v>51786.06</v>
       </c>
       <c r="E11" s="4">
-        <f>IE-D11</f>
+        <f t="shared" si="0"/>
         <v>8033.4979999999996</v>
       </c>
       <c r="H11">
@@ -2041,36 +2048,36 @@
         <v>1806.5380000000005</v>
       </c>
       <c r="N11">
-        <f>Rhc/($H11-N$4)^2</f>
+        <f t="shared" si="1"/>
         <v>1922.2376982705766</v>
       </c>
       <c r="O11">
-        <f>Rhc/($H11-O$4)^2</f>
+        <f t="shared" si="1"/>
         <v>1863.9687270586703</v>
       </c>
       <c r="P11">
-        <f>Rhc/($H11-P$4)^2</f>
-        <v>1851.7262494720326</v>
+        <f t="shared" si="1"/>
+        <v>1851.6979993012762</v>
       </c>
       <c r="Q11">
-        <f>Rhc/($H11-Q$4)^2</f>
-        <v>1846.8973087897073</v>
+        <f t="shared" si="1"/>
+        <v>1846.9259032994748</v>
       </c>
       <c r="S11" s="4">
+        <f t="shared" si="5"/>
+        <v>18.769698270575873</v>
+      </c>
+      <c r="T11" s="4">
+        <f t="shared" si="2"/>
+        <v>16.640727058676248</v>
+      </c>
+      <c r="U11" s="4">
         <f t="shared" si="3"/>
-        <v>18.769698270575873</v>
-      </c>
-      <c r="T11" s="4">
-        <f t="shared" si="0"/>
-        <v>16.640727058676248</v>
-      </c>
-      <c r="U11" s="4">
-        <f t="shared" si="1"/>
-        <v>29.988249472035022</v>
+        <v>29.959999301278685</v>
       </c>
       <c r="V11" s="4">
-        <f t="shared" si="2"/>
-        <v>40.359308789706802</v>
+        <f t="shared" si="4"/>
+        <v>40.387903299474374</v>
       </c>
     </row>
     <row r="12" spans="1:22" x14ac:dyDescent="0.25">
@@ -2084,7 +2091,7 @@
         <v>51916.94</v>
       </c>
       <c r="E12" s="4">
-        <f>IE-D12</f>
+        <f t="shared" si="0"/>
         <v>7902.6179999999949</v>
       </c>
       <c r="H12">
@@ -2100,21 +2107,21 @@
       </c>
       <c r="P12">
         <f>Rhc/($H12-P$4)^2</f>
-        <v>1450.4283799293994</v>
+        <v>1450.4087959516412</v>
       </c>
       <c r="Q12">
         <f>Rhc/($H12-Q$4)^2</f>
-        <v>1447.080045452062</v>
+        <v>1447.0998770078386</v>
       </c>
       <c r="S12" s="4"/>
       <c r="T12" s="4"/>
       <c r="U12" s="4">
-        <f t="shared" si="1"/>
-        <v>38.640379929398932</v>
+        <f t="shared" si="3"/>
+        <v>38.62079595164073</v>
       </c>
       <c r="V12" s="4">
-        <f t="shared" si="2"/>
-        <v>-3.5679545479317767</v>
+        <f t="shared" si="4"/>
+        <v>-3.5481229921551858</v>
       </c>
     </row>
     <row r="13" spans="1:22" x14ac:dyDescent="0.25">
@@ -2125,7 +2132,7 @@
         <v>51944.11</v>
       </c>
       <c r="E13" s="4">
-        <f>IE-D13</f>
+        <f t="shared" si="0"/>
         <v>7875.4479999999967</v>
       </c>
       <c r="N13" s="7">
@@ -2133,16 +2140,16 @@
         <v>104.90626977362112</v>
       </c>
       <c r="O13" s="7">
-        <f t="shared" ref="O13:Q13" si="4">SQRT(SUMXMY2(O6:O12,J6:J12)/COUNT(O6:O12))</f>
+        <f t="shared" ref="O13:Q13" si="6">SQRT(SUMXMY2(O6:O12,J6:J12)/COUNT(O6:O12))</f>
         <v>59.050294705055386</v>
       </c>
       <c r="P13" s="7">
-        <f t="shared" si="4"/>
-        <v>68.102055506481136</v>
+        <f t="shared" si="6"/>
+        <v>68.59198264831781</v>
       </c>
       <c r="Q13" s="7">
-        <f t="shared" si="4"/>
-        <v>69.407151916200405</v>
+        <f t="shared" si="6"/>
+        <v>69.10494631217189</v>
       </c>
       <c r="S13" s="4"/>
       <c r="T13" s="4"/>
@@ -2163,7 +2170,7 @@
         <v>54653.72</v>
       </c>
       <c r="E14" s="4">
-        <f>IE-D14</f>
+        <f t="shared" si="0"/>
         <v>5165.8379999999961</v>
       </c>
       <c r="I14" s="1" t="s">
@@ -2178,7 +2185,7 @@
         <v>54861.81</v>
       </c>
       <c r="E15" s="4">
-        <f>IE-D15</f>
+        <f t="shared" si="0"/>
         <v>4957.7479999999996</v>
       </c>
       <c r="H15" s="1" t="s">
@@ -2208,26 +2215,26 @@
         <v>54928.08</v>
       </c>
       <c r="E16" s="4">
-        <f>IE-D16</f>
+        <f t="shared" si="0"/>
         <v>4891.4779999999955</v>
       </c>
       <c r="H16">
         <v>7</v>
       </c>
       <c r="I16" s="4">
-        <f>$H16-SQRT(Rhc/I6)</f>
+        <f t="shared" ref="I16:L21" si="7">$H16-SQRT(Rhc/I6)</f>
         <v>4.4518674302090959</v>
       </c>
       <c r="J16" s="4">
-        <f>$H16-SQRT(Rhc/J6)</f>
+        <f t="shared" si="7"/>
         <v>4.3321971159956512</v>
       </c>
       <c r="K16" s="4">
-        <f>$H16-SQRT(Rhc/K6)</f>
+        <f t="shared" si="7"/>
         <v>4.3081632281833544</v>
       </c>
       <c r="L16" s="4">
-        <f>$H16-SQRT(Rhc/L6)</f>
+        <f t="shared" si="7"/>
         <v>4.296141527051935</v>
       </c>
     </row>
@@ -2239,26 +2246,26 @@
         <v>54930.11</v>
       </c>
       <c r="E17" s="4">
-        <f>IE-D17</f>
+        <f t="shared" si="0"/>
         <v>4889.4479999999967</v>
       </c>
       <c r="H17">
         <v>8</v>
       </c>
       <c r="I17" s="4">
-        <f>$H17-SQRT(Rhc/I7)</f>
+        <f t="shared" si="7"/>
         <v>4.4066929890986923</v>
       </c>
       <c r="J17" s="4">
-        <f>$H17-SQRT(Rhc/J7)</f>
+        <f t="shared" si="7"/>
         <v>4.3040607737313508</v>
       </c>
       <c r="K17" s="4">
-        <f>$H17-SQRT(Rhc/K7)</f>
+        <f t="shared" si="7"/>
         <v>4.2735811195160966</v>
       </c>
       <c r="L17" s="4">
-        <f>$H17-SQRT(Rhc/L7)</f>
+        <f t="shared" si="7"/>
         <v>4.26715865143073</v>
       </c>
     </row>
@@ -2276,26 +2283,26 @@
         <v>56338.93</v>
       </c>
       <c r="E18" s="4">
-        <f>IE-D18</f>
+        <f t="shared" si="0"/>
         <v>3480.627999999997</v>
       </c>
       <c r="H18">
         <v>9</v>
       </c>
       <c r="I18" s="4">
-        <f>$H18-SQRT(Rhc/I8)</f>
+        <f t="shared" si="7"/>
         <v>4.390999290581993</v>
       </c>
       <c r="J18" s="4">
-        <f>$H18-SQRT(Rhc/J8)</f>
+        <f t="shared" si="7"/>
         <v>4.2952674265654469</v>
       </c>
       <c r="K18" s="4">
-        <f>$H18-SQRT(Rhc/K8)</f>
+        <f t="shared" si="7"/>
         <v>4.263504663935227</v>
       </c>
       <c r="L18" s="4">
-        <f>$H18-SQRT(Rhc/L8)</f>
+        <f t="shared" si="7"/>
         <v>4.2625215173978237</v>
       </c>
     </row>
@@ -2307,91 +2314,94 @@
         <v>56451.03</v>
       </c>
       <c r="E19" s="4">
-        <f>IE-D19</f>
+        <f t="shared" si="0"/>
         <v>3368.5279999999984</v>
       </c>
       <c r="H19">
         <v>10</v>
       </c>
       <c r="I19" s="4">
-        <f>$H19-SQRT(Rhc/I9)</f>
+        <f t="shared" si="7"/>
         <v>4.3850180888125125</v>
       </c>
       <c r="J19" s="4">
-        <f>$H19-SQRT(Rhc/J9)</f>
+        <f t="shared" si="7"/>
         <v>4.2923532637647668</v>
       </c>
       <c r="K19" s="4">
-        <f>$H19-SQRT(Rhc/K9)</f>
+        <f t="shared" si="7"/>
+        <v>4.2718169190627808</v>
+      </c>
+      <c r="L19" s="4">
+        <f t="shared" si="7"/>
         <v>4.2781692375818494</v>
-      </c>
-      <c r="L19" s="4">
-        <f>$H19-SQRT(Rhc/L9)</f>
-        <v>4.2718169190627808</v>
       </c>
     </row>
     <row r="20" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B20" t="s">
         <v>10</v>
       </c>
-      <c r="C20" s="3">
-        <v>1</v>
+      <c r="C20">
+        <v>2</v>
       </c>
       <c r="D20">
         <v>56467.71</v>
       </c>
       <c r="E20" s="4">
-        <f>IE-D20</f>
+        <f t="shared" si="0"/>
         <v>3351.8479999999981</v>
       </c>
       <c r="H20">
         <v>11</v>
       </c>
       <c r="I20" s="4">
-        <f>$H20-SQRT(Rhc/I10)</f>
+        <f t="shared" si="7"/>
         <v>4.3769506725470544</v>
       </c>
       <c r="J20" s="4">
-        <f>$H20-SQRT(Rhc/J10)</f>
+        <f t="shared" si="7"/>
         <v>4.2918936991786927</v>
       </c>
       <c r="K20" s="4">
-        <f>$H20-SQRT(Rhc/K10)</f>
+        <f t="shared" si="7"/>
         <v>4.2237235133597881</v>
       </c>
       <c r="L20" s="4">
-        <f>$H20-SQRT(Rhc/L10)</f>
+        <f t="shared" si="7"/>
         <v>4.4513538033806208</v>
       </c>
     </row>
     <row r="21" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="C21">
-        <v>2</v>
+      <c r="C21" s="3">
+        <v>1</v>
       </c>
       <c r="D21">
         <v>56475.14</v>
       </c>
       <c r="E21" s="4">
-        <f>IE-D21</f>
+        <f t="shared" si="0"/>
         <v>3344.4179999999978</v>
+      </c>
+      <c r="F21" s="3" t="s">
+        <v>31</v>
       </c>
       <c r="H21">
         <v>12</v>
       </c>
       <c r="I21" s="4">
-        <f>$H21-SQRT(Rhc/I11)</f>
+        <f t="shared" si="7"/>
         <v>4.4071577634749142</v>
       </c>
       <c r="J21" s="4">
-        <f>$H21-SQRT(Rhc/J11)</f>
+        <f t="shared" si="7"/>
         <v>4.2926486055896111</v>
       </c>
       <c r="K21" s="4">
-        <f>$H21-SQRT(Rhc/K11)</f>
+        <f t="shared" si="7"/>
         <v>4.2387047023165287</v>
       </c>
       <c r="L21" s="4">
-        <f>$H21-SQRT(Rhc/L11)</f>
+        <f t="shared" si="7"/>
         <v>4.2061217793408652</v>
       </c>
     </row>
@@ -2409,7 +2419,7 @@
         <v>57260.67</v>
       </c>
       <c r="E22" s="4">
-        <f>IE-D22</f>
+        <f t="shared" si="0"/>
         <v>2558.887999999999</v>
       </c>
       <c r="H22">
@@ -2434,7 +2444,7 @@
         <v>57429.7</v>
       </c>
       <c r="E23" s="4">
-        <f>IE-D23</f>
+        <f t="shared" si="0"/>
         <v>2389.8580000000002</v>
       </c>
     </row>
@@ -2449,7 +2459,7 @@
         <v>57317.84</v>
       </c>
       <c r="E24" s="4">
-        <f>IE-D24</f>
+        <f t="shared" si="0"/>
         <v>2501.7180000000008</v>
       </c>
     </row>
@@ -2461,7 +2471,7 @@
         <v>57380.88</v>
       </c>
       <c r="E25" s="4">
-        <f>IE-D25</f>
+        <f t="shared" si="0"/>
         <v>2438.6779999999999</v>
       </c>
     </row>
@@ -2479,7 +2489,7 @@
         <v>57916.09</v>
       </c>
       <c r="E26" s="4">
-        <f>IE-D26</f>
+        <f t="shared" si="0"/>
         <v>1903.4680000000008</v>
       </c>
     </row>
@@ -2491,7 +2501,7 @@
         <v>57972.23</v>
       </c>
       <c r="E27" s="4">
-        <f>IE-D27</f>
+        <f t="shared" si="0"/>
         <v>1847.3279999999941</v>
       </c>
     </row>
@@ -2506,7 +2516,7 @@
         <v>57997.82</v>
       </c>
       <c r="E28" s="4">
-        <f>IE-D28</f>
+        <f t="shared" si="0"/>
         <v>1821.7379999999976</v>
       </c>
     </row>
@@ -2518,7 +2528,7 @@
         <v>58013.02</v>
       </c>
       <c r="E29" s="4">
-        <f>IE-D29</f>
+        <f t="shared" si="0"/>
         <v>1806.5380000000005</v>
       </c>
     </row>
@@ -2536,7 +2546,7 @@
         <v>58368.91</v>
       </c>
       <c r="E30" s="4">
-        <f>IE-D30</f>
+        <f t="shared" si="0"/>
         <v>1450.6479999999938</v>
       </c>
     </row>
@@ -2548,7 +2558,7 @@
         <v>58407.77</v>
       </c>
       <c r="E31" s="4">
-        <f>IE-D31</f>
+        <f t="shared" si="0"/>
         <v>1411.7880000000005</v>
       </c>
     </row>

</xml_diff>